<commit_message>
Add all photos of Ermitaño's productions
</commit_message>
<xml_diff>
--- a/Bodega Dekorarte/Proyectos/Ermitaño/Produccion/Salida de Bodega-Produccion Ermitaño.xlsx
+++ b/Bodega Dekorarte/Proyectos/Ermitaño/Produccion/Salida de Bodega-Produccion Ermitaño.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="33">
   <si>
     <t>NIT. 900,645,501-1</t>
   </si>
@@ -238,6 +238,30 @@
   <si>
     <t>Sombrillas</t>
   </si>
+  <si>
+    <t>Paredes carpas</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Tela</t>
+  </si>
+  <si>
+    <t>Extintor</t>
+  </si>
+  <si>
+    <t>Techo carpa</t>
+  </si>
+  <si>
+    <t>Cintas de peligro</t>
+  </si>
+  <si>
+    <t>Caneca de basura</t>
+  </si>
+  <si>
+    <t>Estructuras carpas</t>
+  </si>
 </sst>
 </file>
 
@@ -375,7 +399,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -538,29 +562,9 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thick">
         <color indexed="64"/>
       </top>
@@ -590,7 +594,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -622,16 +626,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -658,7 +656,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -703,7 +701,7 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -724,7 +722,7 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1648,22 +1646,17 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>208050</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>42450</xdr:rowOff>
     </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1258800</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>1443450</xdr:rowOff>
-    </xdr:to>
+    <xdr:ext cx="1050750" cy="1401000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPr id="22" name="Imagen 21"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1682,8 +1675,575 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="693825" y="25817100"/>
+          <a:off x="693825" y="27293475"/>
           <a:ext cx="1050750" cy="1401000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>26982</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>91647</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1446996</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>1375204</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="512757" y="27342672"/>
+          <a:ext cx="1420014" cy="1283557"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>34821</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>174817</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1427294</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>1330134</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="520596" y="28902217"/>
+          <a:ext cx="1392473" cy="1155317"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>33000</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>71670</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1414277" cy="1356821"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Imagen 23"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="526059" y="30327552"/>
+          <a:ext cx="1414277" cy="1356821"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>212555</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>35757</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1273345</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>1450143</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="521532" y="31892705"/>
+          <a:ext cx="1414386" cy="1060790"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>257080</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>42759</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1280016</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>1443141</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Imagen 24"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742855" y="33199284"/>
+          <a:ext cx="1022936" cy="1400382"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>100996</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>42483</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1346804</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>1458678</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Imagen 25"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="586771" y="34675383"/>
+          <a:ext cx="1245808" cy="1416195"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>221847</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>35446</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1283103</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>1450455</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Imagen 26"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="707622" y="36144721"/>
+          <a:ext cx="1061256" cy="1415009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>35057</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>57756</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1440585</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>1428145</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Imagen 27"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="520832" y="37643406"/>
+          <a:ext cx="1405528" cy="1370389"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>283720</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>43003</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1221231</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>1451470</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Imagen 28"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="534017" y="39340506"/>
+          <a:ext cx="1408467" cy="937511"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>214212</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>33495</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1271687</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>1447881</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Imagen 29"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="521532" y="40750350"/>
+          <a:ext cx="1414386" cy="1057475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>24313</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>107526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1433919</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>1378375</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Imagen 30"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="510088" y="42122301"/>
+          <a:ext cx="1409606" cy="1270849"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>81725</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>36875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1404176</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>1434677</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Imagen 31"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="567500" y="43528025"/>
+          <a:ext cx="1322451" cy="1397802"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>39610</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>168782</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1436960</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>1279019</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Imagen 32"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="525385" y="45136307"/>
+          <a:ext cx="1397350" cy="1110237"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1696,8 +2256,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="B9:H25" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" headerRowCellStyle="Moneda 2">
-  <autoFilter ref="B9:H25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="B9:H38" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" headerRowCellStyle="Moneda 2">
+  <autoFilter ref="B9:H38"/>
   <tableColumns count="7">
     <tableColumn id="1" name="No." dataDxfId="6"/>
     <tableColumn id="2" name="IMAGEN" dataDxfId="5"/>
@@ -1974,10 +2534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H56"/>
+  <dimension ref="B1:H69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28:B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1995,100 +2555,100 @@
   <sheetData>
     <row r="1" spans="2:8" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="103.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="25"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="30"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="28"/>
     </row>
     <row r="4" spans="2:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="42"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="40"/>
     </row>
     <row r="5" spans="2:8" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="36"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="34"/>
     </row>
     <row r="6" spans="2:8" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="39"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="37"/>
     </row>
     <row r="7" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="45"/>
-    </row>
-    <row r="8" spans="2:8" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="31" t="s">
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="43"/>
+    </row>
+    <row r="8" spans="2:8" s="18" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="33"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="31"/>
     </row>
     <row r="9" spans="2:8" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="15" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2103,11 +2663,15 @@
       <c r="E10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="22">
+      <c r="F10" s="20">
         <v>1</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="3"/>
+      <c r="G10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="11" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="10">
@@ -2120,11 +2684,15 @@
       <c r="E11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="20">
         <v>1</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="7"/>
+      <c r="G11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="12" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="10">
@@ -2137,11 +2705,15 @@
       <c r="E12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="19">
         <v>1</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="G12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="13" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="10">
@@ -2154,11 +2726,15 @@
       <c r="E13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="19">
         <v>15</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="14" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="10">
@@ -2171,11 +2747,15 @@
       <c r="E14" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="20">
         <v>1</v>
       </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="7"/>
+      <c r="G14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="15" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="10">
@@ -2188,11 +2768,15 @@
       <c r="E15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="24" t="s">
+      <c r="F15" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="11"/>
+      <c r="G15" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="16" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="10">
@@ -2205,11 +2789,15 @@
       <c r="E16" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="22">
+      <c r="F16" s="20">
         <v>1</v>
       </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="7"/>
+      <c r="G16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="17" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="10">
@@ -2222,11 +2810,15 @@
       <c r="E17" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="22">
+      <c r="F17" s="20">
         <v>1</v>
       </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="7"/>
+      <c r="G17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="18" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="10">
@@ -2239,11 +2831,15 @@
       <c r="E18" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="22">
+      <c r="F18" s="20">
         <v>1</v>
       </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="7"/>
+      <c r="G18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="19" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="10">
@@ -2256,11 +2852,15 @@
       <c r="E19" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="22">
+      <c r="F19" s="20">
         <v>1</v>
       </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="7"/>
+      <c r="G19" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="20" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="10">
@@ -2273,11 +2873,15 @@
       <c r="E20" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="22">
+      <c r="F20" s="20">
         <v>1</v>
       </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="7"/>
+      <c r="G20" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="21" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="10">
@@ -2290,11 +2894,15 @@
       <c r="E21" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="22">
+      <c r="F21" s="20">
         <v>1</v>
       </c>
-      <c r="G21" s="8"/>
-      <c r="H21" s="7"/>
+      <c r="G21" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="22" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="10">
@@ -2307,11 +2915,15 @@
       <c r="E22" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="22">
+      <c r="F22" s="20">
         <v>25</v>
       </c>
-      <c r="G22" s="8"/>
-      <c r="H22" s="7"/>
+      <c r="G22" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="23" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="10">
@@ -2324,69 +2936,305 @@
       <c r="E23" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="22">
+      <c r="F23" s="20">
         <v>3</v>
       </c>
-      <c r="G23" s="8"/>
-      <c r="H23" s="7"/>
+      <c r="G23" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="24" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="10">
         <v>15</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="13" t="s">
+      <c r="C24" s="11"/>
+      <c r="D24" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="23">
+      <c r="F24" s="21">
         <v>5</v>
       </c>
-      <c r="G24" s="13"/>
-      <c r="H24" s="14"/>
+      <c r="G24" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="25" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="10">
         <v>16</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="13" t="s">
+      <c r="C25" s="11"/>
+      <c r="D25" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E25" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="23">
+      <c r="F25" s="21">
         <v>6</v>
       </c>
-      <c r="G25" s="13"/>
-      <c r="H25" s="14"/>
-    </row>
-    <row r="26" spans="2:8" ht="97.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="G25" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="10">
+        <v>17</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="20">
+        <v>4</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="10">
+        <v>18</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="20">
+        <v>4</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="10">
+        <v>19</v>
+      </c>
+      <c r="C28" s="11"/>
+      <c r="D28" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="21">
+        <v>4</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="10">
+        <v>20</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="20">
+        <v>1</v>
+      </c>
+      <c r="G29" s="8"/>
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="10">
+        <v>21</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="20">
+        <v>1</v>
+      </c>
+      <c r="G30" s="8"/>
+      <c r="H30" s="7"/>
+    </row>
+    <row r="31" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="10">
+        <v>22</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="20">
+        <v>1</v>
+      </c>
+      <c r="G31" s="8"/>
+      <c r="H31" s="7"/>
+    </row>
+    <row r="32" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="10">
+        <v>23</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="20">
+        <v>1</v>
+      </c>
+      <c r="G32" s="8"/>
+      <c r="H32" s="7"/>
+    </row>
+    <row r="33" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="10">
+        <v>24</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="20">
+        <v>1</v>
+      </c>
+      <c r="G33" s="8"/>
+      <c r="H33" s="7"/>
+    </row>
+    <row r="34" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="10">
+        <v>25</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="20">
+        <v>1</v>
+      </c>
+      <c r="G34" s="8"/>
+      <c r="H34" s="7"/>
+    </row>
+    <row r="35" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="10">
+        <v>26</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="20">
+        <v>1</v>
+      </c>
+      <c r="G35" s="8"/>
+      <c r="H35" s="7"/>
+    </row>
+    <row r="36" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="10">
+        <v>27</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="20">
+        <v>1</v>
+      </c>
+      <c r="G36" s="8"/>
+      <c r="H36" s="7"/>
+    </row>
+    <row r="37" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="10">
+        <v>28</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="20">
+        <v>1</v>
+      </c>
+      <c r="G37" s="8"/>
+      <c r="H37" s="7"/>
+    </row>
+    <row r="38" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="10">
+        <v>29</v>
+      </c>
+      <c r="C38" s="11"/>
+      <c r="D38" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="21">
+        <v>5</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="97.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="2:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="2:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="2:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="2:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="2:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="2:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="2:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="2:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2395,6 +3243,19 @@
     <row r="54" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="55" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="56" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="97.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="B2:H2"/>

</xml_diff>